<commit_message>
structure learning + model visualisation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NUST 3rd Semester\AI\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NUST 3rd Semester\AI\KTAS-BayesNet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4434B133-1E38-4393-9D9F-9227F89AA994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F06DCC-2E45-4172-B708-E67869FAC808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="945" windowWidth="15375" windowHeight="7875" xr2:uid="{70F6DD15-1D42-45A4-BF89-3681A8406317}"/>
+    <workbookView xWindow="1035" yWindow="1290" windowWidth="15375" windowHeight="7875" xr2:uid="{70F6DD15-1D42-45A4-BF89-3681A8406317}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -1908,14 +1908,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA683E7-4B55-4A99-9D31-54D44BB29D67}">
   <dimension ref="A1:C1267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.140625" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -15768,6 +15769,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:D1267">
+    <sortCondition ref="D1:D1267"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>